<commit_message>
Product Backlog 4, Sprint 4 Planning
</commit_message>
<xml_diff>
--- a/Scrum/Product Backlog.xlsx
+++ b/Scrum/Product Backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jared\Desktop\SEPT\Scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCB3408-A905-4AE8-B673-02776D404BE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F0A338-97A1-44DE-883B-1E25CDFC7608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Calculations" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Product Backlog'!$E$4:$E$63</definedName>
     <definedName name="lstMetrics">OFFSET('Product Backlog'!$C$5:$C$35,0,0,COUNTA('Product Backlog'!$C$5:$C$35))</definedName>
     <definedName name="lstYears">OFFSET('Product Backlog'!$C$4:$I$4,0,1,1,COUNTA('Product Backlog'!$C$4:$I$4)-1)</definedName>
     <definedName name="SelectedYear">#REF!</definedName>
@@ -339,15 +340,9 @@
     <t>As a customer, I want to view my profile page so I can change my password</t>
   </si>
   <si>
-    <t>As a customer, I want to be able to sign in with Twitter, so I do not have to make a new account.</t>
-  </si>
-  <si>
     <t>As a customer, I want to be able to filter my search, so I can find the items I am interested in more easily. </t>
   </si>
   <si>
-    <t>As a customer, I want to be able to press a button to share a book to social media, so I can let people know my opinion.</t>
-  </si>
-  <si>
     <t>As a customer, I want to be able to shut down my account, so that I won't worry about my data being stolen</t>
   </si>
   <si>
@@ -388,6 +383,12 @@
   </si>
   <si>
     <t>As a business user, I want to change my account type to a regular user account, so that I can remove my business' details from my account.</t>
+  </si>
+  <si>
+    <t>As a customer, I want to cancel my order after 2 hours of purchasing, so I can get a full refund.</t>
+  </si>
+  <si>
+    <t>As a business user, I want to be able to upload images to my books, so that I can display previews for each book item.</t>
   </si>
 </sst>
 </file>
@@ -632,7 +633,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -687,9 +688,6 @@
     <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -703,9 +701,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -745,6 +740,9 @@
     </xf>
     <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1205,15 +1203,15 @@
   </sheetPr>
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A56" zoomScaleNormal="100" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="1.75" customWidth="1"/>
     <col min="2" max="2" width="7.125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="67.75" style="33" customWidth="1"/>
+    <col min="3" max="3" width="67.75" style="31" customWidth="1"/>
     <col min="4" max="4" width="24.25" customWidth="1"/>
     <col min="5" max="5" width="9.125" customWidth="1"/>
     <col min="6" max="6" width="18.125" bestFit="1" customWidth="1"/>
@@ -1227,7 +1225,7 @@
     <row r="2" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="11"/>
       <c r="B2" s="12"/>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="32" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="13"/>
@@ -1240,7 +1238,7 @@
     <row r="3" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="11"/>
       <c r="B3" s="12"/>
-      <c r="C3" s="35"/>
+      <c r="C3" s="33"/>
       <c r="D3" s="13"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
@@ -1250,100 +1248,98 @@
     </row>
     <row r="4" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="F4" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="32" t="s">
+      <c r="G4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="32" t="s">
+      <c r="H4" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="32" t="s">
+      <c r="I4" s="30" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1" ht="145.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
       <c r="B5" s="15">
-        <v>3</v>
-      </c>
-      <c r="C5" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>10</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="14"/>
       <c r="E5" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="28">
-        <v>5</v>
+        <v>37</v>
+      </c>
+      <c r="F5" s="26">
+        <v>13</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="H5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="16"/>
+      <c r="I5" s="16" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="6" spans="1:9" s="4" customFormat="1" ht="63.75" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="B6" s="17">
-        <v>4</v>
-      </c>
-      <c r="C6" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>10</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="14"/>
       <c r="E6" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="29">
+        <v>40</v>
+      </c>
+      <c r="F6" s="27">
         <v>5</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="H6" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="18"/>
+      <c r="I6" s="18" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="7" spans="1:9" s="4" customFormat="1" ht="63.75" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="17">
-        <v>5</v>
-      </c>
-      <c r="C7" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" s="29">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="27">
+        <v>3</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="H7" s="16" t="s">
         <v>13</v>
@@ -1353,47 +1349,43 @@
     <row r="8" spans="1:9" s="4" customFormat="1" ht="63.75" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="17">
-        <v>6</v>
-      </c>
-      <c r="C8" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="29">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="27">
+        <v>3</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="H8" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="21"/>
+      <c r="I8" s="18"/>
     </row>
     <row r="9" spans="1:9" s="4" customFormat="1" ht="63.75" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="17">
-        <v>7</v>
-      </c>
-      <c r="C9" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="29">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="27">
+        <v>3</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="H9" s="16" t="s">
         <v>13</v>
@@ -1403,182 +1395,168 @@
     <row r="10" spans="1:9" s="4" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="B10" s="17">
-        <v>31</v>
-      </c>
-      <c r="C10" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="29">
-        <v>8</v>
+      <c r="C10" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="27">
+        <v>3</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="H10" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="18" t="s">
-        <v>21</v>
-      </c>
+      <c r="I10" s="18"/>
     </row>
     <row r="11" spans="1:9" s="4" customFormat="1" ht="63.75" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="17">
-        <v>32</v>
-      </c>
-      <c r="C11" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>20</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="14"/>
       <c r="E11" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="29">
-        <v>5</v>
+        <v>40</v>
+      </c>
+      <c r="F11" s="27">
+        <v>13</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="H11" s="16" t="s">
         <v>13</v>
       </c>
       <c r="I11" s="18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" s="4" customFormat="1" ht="63.75" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="4" customFormat="1" ht="76.5" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="B12" s="15">
-        <v>42</v>
-      </c>
-      <c r="C12" s="38" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>20</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="14"/>
       <c r="E12" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="F12" s="29">
-        <v>3</v>
+        <v>40</v>
+      </c>
+      <c r="F12" s="27">
+        <v>5</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="H12" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="26" t="s">
-        <v>25</v>
+      <c r="I12" s="21" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="4" customFormat="1" ht="63.75" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
-      <c r="B13" s="17">
-        <v>2</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>27</v>
-      </c>
+      <c r="B13" s="22">
+        <v>48</v>
+      </c>
+      <c r="C13" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="14"/>
       <c r="E13" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="29">
+        <v>40</v>
+      </c>
+      <c r="F13" s="27">
         <v>5</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="H13" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I13" s="18"/>
+      <c r="I13" s="18" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="14" spans="1:9" s="4" customFormat="1" ht="63.75" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="15">
-        <v>22</v>
-      </c>
-      <c r="C14" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>27</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" s="14"/>
       <c r="E14" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="29">
+        <v>40</v>
+      </c>
+      <c r="F14" s="27">
         <v>5</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="H14" s="16" t="s">
         <v>13</v>
       </c>
       <c r="I14" s="18" t="s">
-        <v>29</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="4" customFormat="1" ht="63.75" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
-      <c r="B15" s="17">
-        <v>45</v>
-      </c>
-      <c r="C15" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>27</v>
-      </c>
+      <c r="B15" s="22">
+        <v>50</v>
+      </c>
+      <c r="C15" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="D15" s="14"/>
       <c r="E15" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="29">
-        <v>8</v>
+        <v>40</v>
+      </c>
+      <c r="F15" s="27">
+        <v>3</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="H15" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="24" t="s">
-        <v>31</v>
+      <c r="I15" s="18" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="4" customFormat="1" ht="162.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="17">
-        <v>25</v>
-      </c>
-      <c r="C16" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>33</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="D16" s="14"/>
       <c r="E16" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="F16" s="29">
-        <v>3</v>
+        <v>40</v>
+      </c>
+      <c r="F16" s="27">
+        <v>5</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="H16" s="16" t="s">
         <v>13</v>
@@ -1587,23 +1565,21 @@
     </row>
     <row r="17" spans="1:9" s="4" customFormat="1" ht="216" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
-      <c r="B17" s="17">
-        <v>29</v>
-      </c>
-      <c r="C17" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="F17" s="29">
-        <v>5</v>
+      <c r="B17" s="22">
+        <v>55</v>
+      </c>
+      <c r="C17" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="D17" s="14"/>
+      <c r="E17" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="27">
+        <v>13</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="H17" s="16" t="s">
         <v>13</v>
@@ -1612,23 +1588,23 @@
     </row>
     <row r="18" spans="1:9" s="4" customFormat="1" ht="63.75" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
-      <c r="B18" s="17">
-        <v>51</v>
-      </c>
-      <c r="C18" s="38" t="s">
-        <v>35</v>
+      <c r="B18" s="22">
+        <v>14</v>
+      </c>
+      <c r="C18" s="36" t="s">
+        <v>49</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>33</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="29">
-        <v>5</v>
+        <v>50</v>
+      </c>
+      <c r="F18" s="27">
+        <v>3</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="H18" s="16" t="s">
         <v>13</v>
@@ -1638,17 +1614,19 @@
     <row r="19" spans="1:9" s="4" customFormat="1" ht="63.75" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="15">
-        <v>1</v>
-      </c>
-      <c r="C19" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="14"/>
+        <v>26</v>
+      </c>
+      <c r="C19" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>17</v>
+      </c>
       <c r="E19" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="F19" s="29">
-        <v>21</v>
+        <v>50</v>
+      </c>
+      <c r="F19" s="27">
+        <v>8</v>
       </c>
       <c r="G19" s="16" t="s">
         <v>12</v>
@@ -1656,24 +1634,24 @@
       <c r="H19" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I19" s="18" t="s">
-        <v>38</v>
-      </c>
+      <c r="I19" s="18"/>
     </row>
     <row r="20" spans="1:9" s="4" customFormat="1" ht="63.75" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="17">
+        <v>27</v>
+      </c>
+      <c r="C20" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="27">
         <v>8</v>
-      </c>
-      <c r="C20" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20" s="29">
-        <v>3</v>
       </c>
       <c r="G20" s="16" t="s">
         <v>12</v>
@@ -1681,22 +1659,24 @@
       <c r="H20" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I20" s="18"/>
+      <c r="I20" s="21"/>
     </row>
     <row r="21" spans="1:9" s="4" customFormat="1" ht="63.75" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="15">
-        <v>9</v>
-      </c>
-      <c r="C21" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" s="14"/>
-      <c r="E21" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="F21" s="29">
-        <v>13</v>
+        <v>28</v>
+      </c>
+      <c r="C21" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" s="27">
+        <v>8</v>
       </c>
       <c r="G21" s="16" t="s">
         <v>12</v>
@@ -1709,17 +1689,19 @@
     <row r="22" spans="1:9" s="4" customFormat="1" ht="149.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="17">
-        <v>10</v>
-      </c>
-      <c r="C22" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="D22" s="14"/>
-      <c r="E22" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="F22" s="29">
-        <v>13</v>
+        <v>30</v>
+      </c>
+      <c r="C22" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" s="27">
+        <v>5</v>
       </c>
       <c r="G22" s="16" t="s">
         <v>12</v>
@@ -1732,16 +1714,18 @@
     <row r="23" spans="1:9" s="4" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="17">
-        <v>11</v>
-      </c>
-      <c r="C23" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="F23" s="29">
+        <v>36</v>
+      </c>
+      <c r="C23" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F23" s="27">
         <v>3</v>
       </c>
       <c r="G23" s="16" t="s">
@@ -1755,73 +1739,73 @@
     <row r="24" spans="1:9" ht="121.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11"/>
       <c r="B24" s="17">
+        <v>37</v>
+      </c>
+      <c r="C24" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" s="27">
+        <v>3</v>
+      </c>
+      <c r="G24" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="F24" s="29">
-        <v>3</v>
-      </c>
-      <c r="G24" s="16" t="s">
-        <v>112</v>
-      </c>
       <c r="H24" s="16" t="s">
         <v>13</v>
       </c>
       <c r="I24" s="18" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="138.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11"/>
       <c r="B25" s="15">
-        <v>13</v>
-      </c>
-      <c r="C25" s="38" t="s">
-        <v>47</v>
+        <v>38</v>
+      </c>
+      <c r="C25" s="36" t="s">
+        <v>76</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="F25" s="29">
+        <v>50</v>
+      </c>
+      <c r="F25" s="27">
         <v>3</v>
       </c>
       <c r="G25" s="16" t="s">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="H25" s="16" t="s">
         <v>13</v>
       </c>
       <c r="I25" s="18" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="141.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11"/>
-      <c r="B26" s="23">
-        <v>14</v>
-      </c>
-      <c r="C26" s="38" t="s">
-        <v>49</v>
+      <c r="B26" s="17">
+        <v>44</v>
+      </c>
+      <c r="C26" s="36" t="s">
+        <v>86</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E26" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="F26" s="29">
-        <v>3</v>
+      <c r="F26" s="27">
+        <v>5</v>
       </c>
       <c r="G26" s="16" t="s">
         <v>12</v>
@@ -1829,52 +1813,56 @@
       <c r="H26" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I26" s="18"/>
+      <c r="I26" s="18" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="27" spans="1:9" ht="63.75" x14ac:dyDescent="0.3">
       <c r="A27" s="11"/>
       <c r="B27" s="15">
-        <v>15</v>
-      </c>
-      <c r="C27" s="38" t="s">
-        <v>51</v>
+        <v>46</v>
+      </c>
+      <c r="C27" s="36" t="s">
+        <v>88</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="F27" s="29">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="F27" s="27">
+        <v>5</v>
       </c>
       <c r="G27" s="16" t="s">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="H27" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I27" s="18"/>
+      <c r="I27" s="18" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="28" spans="1:9" ht="63.75" x14ac:dyDescent="0.3">
       <c r="A28" s="11"/>
       <c r="B28" s="17">
-        <v>16</v>
-      </c>
-      <c r="C28" s="38" t="s">
-        <v>52</v>
+        <v>54</v>
+      </c>
+      <c r="C28" s="36" t="s">
+        <v>99</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="F28" s="29">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="F28" s="27">
+        <v>3</v>
       </c>
       <c r="G28" s="16" t="s">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="H28" s="16" t="s">
         <v>13</v>
@@ -1883,156 +1871,150 @@
     </row>
     <row r="29" spans="1:9" ht="63.75" x14ac:dyDescent="0.3">
       <c r="A29" s="11"/>
-      <c r="B29" s="17">
-        <v>17</v>
-      </c>
-      <c r="C29" s="38" t="s">
-        <v>53</v>
+      <c r="B29" s="22">
+        <v>56</v>
+      </c>
+      <c r="C29" s="36" t="s">
+        <v>100</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="F29" s="29">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="F29" s="27">
+        <v>3</v>
       </c>
       <c r="G29" s="16" t="s">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="H29" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I29" s="18"/>
+      <c r="I29" s="21"/>
     </row>
     <row r="30" spans="1:9" ht="63.75" x14ac:dyDescent="0.3">
       <c r="A30" s="11"/>
-      <c r="B30" s="17">
-        <v>18</v>
-      </c>
-      <c r="C30" s="39" t="s">
-        <v>54</v>
+      <c r="B30" s="22">
+        <v>59</v>
+      </c>
+      <c r="C30" s="36" t="s">
+        <v>112</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="F30" s="29">
+        <v>50</v>
+      </c>
+      <c r="F30" s="27">
         <v>3</v>
       </c>
       <c r="G30" s="16" t="s">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="H30" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I30" s="18" t="s">
-        <v>55</v>
-      </c>
+      <c r="I30" s="21"/>
     </row>
     <row r="31" spans="1:9" ht="63.75" x14ac:dyDescent="0.3">
       <c r="A31" s="11"/>
       <c r="B31" s="15">
-        <v>19</v>
-      </c>
-      <c r="C31" s="38" t="s">
-        <v>56</v>
+        <v>5</v>
+      </c>
+      <c r="C31" s="36" t="s">
+        <v>15</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E31" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F31" s="29">
-        <v>3</v>
+      <c r="F31" s="27">
+        <v>5</v>
       </c>
       <c r="G31" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H31" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I31" s="18" t="s">
-        <v>57</v>
-      </c>
+      <c r="I31" s="18"/>
     </row>
     <row r="32" spans="1:9" ht="63.75" x14ac:dyDescent="0.3">
       <c r="A32" s="11"/>
-      <c r="B32" s="23">
-        <v>20</v>
-      </c>
-      <c r="C32" s="38" t="s">
-        <v>58</v>
+      <c r="B32" s="17">
+        <v>6</v>
+      </c>
+      <c r="C32" s="36" t="s">
+        <v>16</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="E32" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F32" s="29">
-        <v>3</v>
+      <c r="F32" s="27">
+        <v>13</v>
       </c>
       <c r="G32" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H32" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I32" s="18" t="s">
-        <v>59</v>
-      </c>
+      <c r="I32" s="20"/>
     </row>
     <row r="33" spans="1:9" ht="63.75" x14ac:dyDescent="0.3">
       <c r="A33" s="11"/>
       <c r="B33" s="15">
-        <v>21</v>
-      </c>
-      <c r="C33" s="40" t="s">
-        <v>60</v>
+        <v>42</v>
+      </c>
+      <c r="C33" s="36" t="s">
+        <v>24</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E33" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F33" s="30">
-        <v>8</v>
+      <c r="F33" s="28">
+        <v>3</v>
       </c>
       <c r="G33" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H33" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I33" s="20" t="s">
-        <v>61</v>
+      <c r="I33" s="39" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="63.75" x14ac:dyDescent="0.3">
       <c r="A34" s="11"/>
       <c r="B34" s="17">
-        <v>23</v>
-      </c>
-      <c r="C34" s="38" t="s">
-        <v>62</v>
+        <v>25</v>
+      </c>
+      <c r="C34" s="36" t="s">
+        <v>32</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="E34" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F34" s="29">
-        <v>13</v>
+      <c r="F34" s="27">
+        <v>3</v>
       </c>
       <c r="G34" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H34" s="16" t="s">
         <v>13</v>
@@ -2042,22 +2024,22 @@
     <row r="35" spans="1:9" ht="81.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="11"/>
       <c r="B35" s="17">
-        <v>24</v>
-      </c>
-      <c r="C35" s="38" t="s">
-        <v>63</v>
+        <v>29</v>
+      </c>
+      <c r="C35" s="36" t="s">
+        <v>34</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E35" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="F35" s="29">
-        <v>1</v>
+      <c r="F35" s="27">
+        <v>5</v>
       </c>
       <c r="G35" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H35" s="16" t="s">
         <v>13</v>
@@ -2067,72 +2049,76 @@
     <row r="36" spans="1:9" ht="81" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="11"/>
       <c r="B36" s="17">
-        <v>26</v>
-      </c>
-      <c r="C36" s="38" t="s">
-        <v>64</v>
+        <v>12</v>
+      </c>
+      <c r="C36" s="36" t="s">
+        <v>44</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="F36" s="29">
-        <v>8</v>
+        <v>45</v>
+      </c>
+      <c r="F36" s="27">
+        <v>3</v>
       </c>
       <c r="G36" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H36" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I36" s="18"/>
+      <c r="I36" s="18" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="37" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="11"/>
       <c r="B37" s="15">
-        <v>27</v>
-      </c>
-      <c r="C37" s="38" t="s">
-        <v>65</v>
+        <v>13</v>
+      </c>
+      <c r="C37" s="36" t="s">
+        <v>47</v>
       </c>
       <c r="D37" s="14" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="F37" s="29">
-        <v>8</v>
+        <v>45</v>
+      </c>
+      <c r="F37" s="27">
+        <v>3</v>
       </c>
       <c r="G37" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H37" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I37" s="22"/>
+      <c r="I37" s="18" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="38" spans="1:9" ht="63.75" x14ac:dyDescent="0.3">
       <c r="A38" s="11"/>
       <c r="B38" s="17">
-        <v>28</v>
-      </c>
-      <c r="C38" s="38" t="s">
-        <v>66</v>
+        <v>15</v>
+      </c>
+      <c r="C38" s="36" t="s">
+        <v>51</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="F38" s="29">
-        <v>8</v>
+        <v>45</v>
+      </c>
+      <c r="F38" s="27">
+        <v>1</v>
       </c>
       <c r="G38" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H38" s="16" t="s">
         <v>13</v>
@@ -2142,22 +2128,22 @@
     <row r="39" spans="1:9" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="11"/>
       <c r="B39" s="15">
-        <v>30</v>
-      </c>
-      <c r="C39" s="38" t="s">
-        <v>67</v>
+        <v>16</v>
+      </c>
+      <c r="C39" s="36" t="s">
+        <v>52</v>
       </c>
       <c r="D39" s="14" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="F39" s="29">
-        <v>5</v>
+        <v>45</v>
+      </c>
+      <c r="F39" s="27">
+        <v>1</v>
       </c>
       <c r="G39" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H39" s="16" t="s">
         <v>13</v>
@@ -2167,197 +2153,193 @@
     <row r="40" spans="1:9" ht="75.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="11"/>
       <c r="B40" s="17">
-        <v>33</v>
-      </c>
-      <c r="C40" s="38" t="s">
-        <v>68</v>
+        <v>17</v>
+      </c>
+      <c r="C40" s="36" t="s">
+        <v>53</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E40" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F40" s="29">
-        <v>3</v>
+      <c r="F40" s="27">
+        <v>1</v>
       </c>
       <c r="G40" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H40" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I40" s="18" t="s">
-        <v>69</v>
-      </c>
+      <c r="I40" s="18"/>
     </row>
     <row r="41" spans="1:9" ht="63.75" x14ac:dyDescent="0.3">
       <c r="A41" s="11"/>
       <c r="B41" s="17">
-        <v>34</v>
-      </c>
-      <c r="C41" s="38" t="s">
-        <v>70</v>
+        <v>18</v>
+      </c>
+      <c r="C41" s="37" t="s">
+        <v>54</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E41" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F41" s="29">
+      <c r="F41" s="27">
         <v>3</v>
       </c>
       <c r="G41" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H41" s="16" t="s">
         <v>13</v>
       </c>
       <c r="I41" s="18" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="63.75" x14ac:dyDescent="0.3">
       <c r="A42" s="11"/>
       <c r="B42" s="17">
-        <v>35</v>
-      </c>
-      <c r="C42" s="38" t="s">
-        <v>72</v>
+        <v>19</v>
+      </c>
+      <c r="C42" s="36" t="s">
+        <v>56</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="E42" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F42" s="29">
+      <c r="F42" s="27">
         <v>3</v>
       </c>
       <c r="G42" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H42" s="16" t="s">
         <v>13</v>
       </c>
       <c r="I42" s="18" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="63.75" x14ac:dyDescent="0.3">
       <c r="A43" s="11"/>
       <c r="B43" s="15">
-        <v>36</v>
-      </c>
-      <c r="C43" s="38" t="s">
-        <v>115</v>
+        <v>20</v>
+      </c>
+      <c r="C43" s="36" t="s">
+        <v>58</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="E43" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="F43" s="29">
+        <v>45</v>
+      </c>
+      <c r="F43" s="27">
         <v>3</v>
       </c>
       <c r="G43" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H43" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I43" s="18"/>
+      <c r="I43" s="18" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="44" spans="1:9" ht="63.75" x14ac:dyDescent="0.3">
       <c r="A44" s="11"/>
       <c r="B44" s="17">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="C44" s="38" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="F44" s="29">
-        <v>3</v>
+        <v>45</v>
+      </c>
+      <c r="F44" s="27">
+        <v>8</v>
       </c>
       <c r="G44" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H44" s="16" t="s">
         <v>13</v>
       </c>
       <c r="I44" s="18" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="11"/>
       <c r="B45" s="15">
-        <v>38</v>
-      </c>
-      <c r="C45" s="38" t="s">
-        <v>76</v>
+        <v>23</v>
+      </c>
+      <c r="C45" s="36" t="s">
+        <v>62</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="F45" s="29">
-        <v>3</v>
+        <v>45</v>
+      </c>
+      <c r="F45" s="27">
+        <v>13</v>
       </c>
       <c r="G45" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H45" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I45" s="18" t="s">
-        <v>77</v>
-      </c>
+      <c r="I45" s="18"/>
     </row>
     <row r="46" spans="1:9" ht="63.75" x14ac:dyDescent="0.3">
       <c r="A46" s="11"/>
       <c r="B46" s="17">
-        <v>39</v>
-      </c>
-      <c r="C46" s="38" t="s">
-        <v>78</v>
+        <v>24</v>
+      </c>
+      <c r="C46" s="36" t="s">
+        <v>63</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E46" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F46" s="29">
-        <v>3</v>
+      <c r="F46" s="27">
+        <v>1</v>
       </c>
       <c r="G46" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H46" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I46" s="18" t="s">
-        <v>79</v>
-      </c>
+      <c r="I46" s="18"/>
     </row>
     <row r="47" spans="1:9" ht="63.75" x14ac:dyDescent="0.3">
       <c r="A47" s="11"/>
       <c r="B47" s="17">
-        <v>40</v>
-      </c>
-      <c r="C47" s="38" t="s">
-        <v>80</v>
+        <v>33</v>
+      </c>
+      <c r="C47" s="36" t="s">
+        <v>68</v>
       </c>
       <c r="D47" s="14" t="s">
         <v>27</v>
@@ -2365,237 +2347,241 @@
       <c r="E47" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F47" s="29">
+      <c r="F47" s="27">
         <v>3</v>
       </c>
       <c r="G47" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H47" s="16" t="s">
         <v>13</v>
       </c>
       <c r="I47" s="18" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="63.75" x14ac:dyDescent="0.3">
       <c r="A48" s="11"/>
       <c r="B48" s="17">
-        <v>41</v>
-      </c>
-      <c r="C48" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="D48" s="14"/>
+        <v>34</v>
+      </c>
+      <c r="C48" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>27</v>
+      </c>
       <c r="E48" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="F48" s="29">
-        <v>21</v>
+        <v>45</v>
+      </c>
+      <c r="F48" s="27">
+        <v>3</v>
       </c>
       <c r="G48" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H48" s="16" t="s">
         <v>13</v>
       </c>
       <c r="I48" s="18" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="63.75" x14ac:dyDescent="0.3">
       <c r="A49" s="11"/>
       <c r="B49" s="17">
-        <v>43</v>
-      </c>
-      <c r="C49" s="38" t="s">
-        <v>84</v>
+        <v>35</v>
+      </c>
+      <c r="C49" s="36" t="s">
+        <v>72</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="E49" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F49" s="29">
+      <c r="F49" s="27">
         <v>3</v>
       </c>
       <c r="G49" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H49" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I49" s="25" t="s">
-        <v>85</v>
+      <c r="I49" s="18" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="63.75" x14ac:dyDescent="0.3">
       <c r="B50" s="17">
-        <v>44</v>
-      </c>
-      <c r="C50" s="38" t="s">
-        <v>86</v>
+        <v>39</v>
+      </c>
+      <c r="C50" s="36" t="s">
+        <v>78</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E50" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="F50" s="29">
-        <v>5</v>
+        <v>45</v>
+      </c>
+      <c r="F50" s="27">
+        <v>3</v>
       </c>
       <c r="G50" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H50" s="16" t="s">
         <v>13</v>
       </c>
       <c r="I50" s="18" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" s="17">
-        <v>46</v>
-      </c>
-      <c r="C51" s="38" t="s">
-        <v>88</v>
+        <v>40</v>
+      </c>
+      <c r="C51" s="36" t="s">
+        <v>80</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E51" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="F51" s="29">
+        <v>45</v>
+      </c>
+      <c r="F51" s="27">
+        <v>3</v>
+      </c>
+      <c r="G51" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="H51" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I51" s="18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="63.75" x14ac:dyDescent="0.3">
+      <c r="B52" s="17">
+        <v>43</v>
+      </c>
+      <c r="C52" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="D52" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E52" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="F52" s="27">
+        <v>3</v>
+      </c>
+      <c r="G52" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="H52" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I52" s="24" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="63.75" x14ac:dyDescent="0.3">
+      <c r="B53" s="17">
+        <v>52</v>
+      </c>
+      <c r="C53" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="D53" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="E53" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="F53" s="27">
         <v>5</v>
       </c>
-      <c r="G51" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="H51" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="I51" s="18" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="76.5" x14ac:dyDescent="0.3">
-      <c r="B52" s="23">
-        <v>47</v>
-      </c>
-      <c r="C52" s="38" t="s">
-        <v>90</v>
-      </c>
-      <c r="D52" s="14"/>
-      <c r="E52" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="F52" s="29">
-        <v>13</v>
-      </c>
-      <c r="G52" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="H52" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="I52" s="22" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="63.75" x14ac:dyDescent="0.3">
-      <c r="B53" s="23">
-        <v>48</v>
-      </c>
-      <c r="C53" s="38" t="s">
-        <v>92</v>
-      </c>
-      <c r="D53" s="14"/>
-      <c r="E53" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="F53" s="29">
-        <v>13</v>
-      </c>
       <c r="G53" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H53" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I53" s="18" t="s">
-        <v>93</v>
-      </c>
+      <c r="I53" s="18"/>
     </row>
     <row r="54" spans="1:9" ht="63.75" x14ac:dyDescent="0.3">
-      <c r="B54" s="23">
-        <v>49</v>
-      </c>
-      <c r="C54" s="38" t="s">
-        <v>94</v>
-      </c>
-      <c r="D54" s="14"/>
+      <c r="B54" s="22">
+        <v>58</v>
+      </c>
+      <c r="C54" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="D54" s="14" t="s">
+        <v>27</v>
+      </c>
       <c r="E54" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="F54" s="29">
-        <v>13</v>
+        <v>45</v>
+      </c>
+      <c r="F54" s="27">
+        <v>3</v>
       </c>
       <c r="G54" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H54" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I54" s="18" t="s">
-        <v>95</v>
-      </c>
+      <c r="I54" s="21"/>
     </row>
     <row r="55" spans="1:9" ht="63.75" x14ac:dyDescent="0.3">
-      <c r="B55" s="23">
-        <v>50</v>
-      </c>
-      <c r="C55" s="38" t="s">
-        <v>96</v>
-      </c>
-      <c r="D55" s="14"/>
+      <c r="B55" s="17">
+        <v>3</v>
+      </c>
+      <c r="C55" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" s="14" t="s">
+        <v>10</v>
+      </c>
       <c r="E55" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="F55" s="29">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="F55" s="27">
+        <v>5</v>
       </c>
       <c r="G55" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H55" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I55" s="18" t="s">
-        <v>97</v>
-      </c>
+      <c r="I55" s="18"/>
     </row>
     <row r="56" spans="1:9" ht="63.75" x14ac:dyDescent="0.3">
       <c r="B56" s="17">
-        <v>52</v>
-      </c>
-      <c r="C56" s="38" t="s">
-        <v>98</v>
+        <v>4</v>
+      </c>
+      <c r="C56" s="36" t="s">
+        <v>14</v>
       </c>
       <c r="D56" s="14" t="s">
-        <v>113</v>
+        <v>10</v>
       </c>
       <c r="E56" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="F56" s="29">
+        <v>11</v>
+      </c>
+      <c r="F56" s="27">
         <v>5</v>
       </c>
       <c r="G56" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H56" s="16" t="s">
         <v>13</v>
@@ -2604,174 +2590,187 @@
     </row>
     <row r="57" spans="1:9" ht="63.75" x14ac:dyDescent="0.3">
       <c r="B57" s="17">
-        <v>53</v>
-      </c>
-      <c r="C57" s="38" t="s">
-        <v>99</v>
-      </c>
-      <c r="D57" s="14"/>
+        <v>7</v>
+      </c>
+      <c r="C57" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57" s="14" t="s">
+        <v>17</v>
+      </c>
       <c r="E57" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="F57" s="29">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="F57" s="27">
+        <v>5</v>
       </c>
       <c r="G57" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H57" s="16" t="s">
         <v>13</v>
       </c>
       <c r="I57" s="18"/>
     </row>
-    <row r="58" spans="1:9" ht="63.75" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" ht="76.5" x14ac:dyDescent="0.3">
       <c r="B58" s="17">
-        <v>54</v>
-      </c>
-      <c r="C58" s="38" t="s">
-        <v>100</v>
+        <v>31</v>
+      </c>
+      <c r="C58" s="36" t="s">
+        <v>19</v>
       </c>
       <c r="D58" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E58" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F58" s="27">
+        <v>8</v>
+      </c>
+      <c r="G58" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="H58" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I58" s="18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="63.75" x14ac:dyDescent="0.3">
+      <c r="B59" s="17">
+        <v>32</v>
+      </c>
+      <c r="C59" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D59" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E59" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F59" s="27">
+        <v>5</v>
+      </c>
+      <c r="G59" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="H59" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I59" s="18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="63.75" x14ac:dyDescent="0.3">
+      <c r="B60" s="17">
+        <v>2</v>
+      </c>
+      <c r="C60" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D60" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="E58" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="F58" s="29">
-        <v>3</v>
-      </c>
-      <c r="G58" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="H58" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="I58" s="18"/>
-    </row>
-    <row r="59" spans="1:9" ht="63.75" x14ac:dyDescent="0.3">
-      <c r="B59" s="23">
-        <v>55</v>
-      </c>
-      <c r="C59" s="38" t="s">
-        <v>101</v>
-      </c>
-      <c r="D59" s="14"/>
-      <c r="E59" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="F59" s="29">
-        <v>13</v>
-      </c>
-      <c r="G59" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="H59" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="I59" s="18"/>
-    </row>
-    <row r="60" spans="1:9" ht="63.75" x14ac:dyDescent="0.3">
-      <c r="B60" s="23">
-        <v>56</v>
-      </c>
-      <c r="C60" s="38" t="s">
-        <v>102</v>
-      </c>
-      <c r="D60" s="14" t="s">
-        <v>10</v>
-      </c>
       <c r="E60" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="F60" s="29">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="F60" s="27">
+        <v>5</v>
       </c>
       <c r="G60" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H60" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I60" s="22"/>
+      <c r="I60" s="18"/>
     </row>
     <row r="61" spans="1:9" ht="63.75" x14ac:dyDescent="0.3">
-      <c r="B61" s="23">
-        <v>57</v>
-      </c>
-      <c r="C61" s="38" t="s">
-        <v>103</v>
-      </c>
-      <c r="D61" s="14"/>
+      <c r="B61" s="17">
+        <v>22</v>
+      </c>
+      <c r="C61" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="D61" s="14" t="s">
+        <v>27</v>
+      </c>
       <c r="E61" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="F61" s="29">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="F61" s="27">
+        <v>5</v>
       </c>
       <c r="G61" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H61" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I61" s="22" t="s">
-        <v>104</v>
+      <c r="I61" s="18" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="63.75" x14ac:dyDescent="0.3">
-      <c r="B62" s="23">
-        <v>58</v>
-      </c>
-      <c r="C62" s="38" t="s">
-        <v>105</v>
+      <c r="B62" s="17">
+        <v>45</v>
+      </c>
+      <c r="C62" s="36" t="s">
+        <v>30</v>
       </c>
       <c r="D62" s="14" t="s">
         <v>27</v>
       </c>
       <c r="E62" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="F62" s="29">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="F62" s="27">
+        <v>8</v>
       </c>
       <c r="G62" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H62" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I62" s="22"/>
+      <c r="I62" s="23" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="63" spans="1:9" ht="63.75" x14ac:dyDescent="0.3">
-      <c r="B63" s="23">
-        <v>59</v>
-      </c>
-      <c r="C63" s="38" t="s">
-        <v>114</v>
+      <c r="B63" s="17">
+        <v>51</v>
+      </c>
+      <c r="C63" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="D63" s="14" t="s">
         <v>33</v>
       </c>
       <c r="E63" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="F63" s="29">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="F63" s="27">
+        <v>5</v>
       </c>
       <c r="G63" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H63" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I63" s="22"/>
+      <c r="I63" s="18"/>
     </row>
     <row r="66" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F66" s="27"/>
+      <c r="F66" s="25"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:I61">
-    <sortCondition ref="D5:D61"/>
+  <autoFilter ref="E4:E63" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:I63">
+    <sortCondition descending="1" ref="E5:E63"/>
   </sortState>
   <conditionalFormatting sqref="B5:C5 B6:B60 I48 I50 H5:I15 C60:F60 C27:C59 I16:I46 I52:I60 C7:C24 H16:H60 D5:F59">
     <cfRule type="expression" dxfId="10" priority="32">
@@ -2847,17 +2846,17 @@
   <sheetData>
     <row r="1" spans="1:8" s="7" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D2" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C3" s="2" t="e">
         <f>SelectedYear</f>
@@ -2870,7 +2869,7 @@
     </row>
     <row r="4" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C4" s="2" t="e">
         <f>C3-1</f>
@@ -2884,7 +2883,7 @@
     <row r="5" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C6" s="1" t="e">
         <f ca="1">MATCH(C7,lstYears,0)+1</f>
@@ -2909,7 +2908,7 @@
     </row>
     <row r="7" spans="1:8" ht="23.25" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B7" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C7" s="9" t="e">
         <f>D7-1</f>
@@ -3106,7 +3105,7 @@
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="1:8" ht="23.25" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B14" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -3122,7 +3121,7 @@
       </c>
       <c r="B15" t="str">
         <f>IF('Product Backlog'!C5=0,"",'Product Backlog'!C5)</f>
-        <v>As an Admin, I want to view all current users, so that I can see all user information.</v>
+        <v>As a seller, I want to be able to provide incentive for frequent buyers, so that they spend more money on my store.</v>
       </c>
       <c r="C15" t="e">
         <f ca="1">IF(B15="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$33,$A15,C$6),NA()))</f>
@@ -3152,7 +3151,7 @@
       </c>
       <c r="B16" t="str">
         <f>IF('Product Backlog'!C6=0,"",'Product Backlog'!C6)</f>
-        <v>As an Admin, I want to modify user accounts, so that I can edit user information.</v>
+        <v>As a developer for a different website, I want to be able to access the BOOKEROO API so that I can display information from the BOOKEROO API</v>
       </c>
       <c r="C16" t="e">
         <f ca="1">IF(B16="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$33,$A16,C$6),NA()))</f>
@@ -3182,7 +3181,7 @@
       </c>
       <c r="B17" t="str">
         <f>IF('Product Backlog'!C7=0,"",'Product Backlog'!C7)</f>
-        <v>As an Admin, I want to modify users, so that I can suspend/unsuspend users from their account.</v>
+        <v>As an Admin, I want to see the transaction history of an item so I know if the right amount of money is being transferred</v>
       </c>
       <c r="C17" t="e">
         <f ca="1">IF(B17="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$33,$A17,C$6),NA()))</f>
@@ -3212,7 +3211,7 @@
       </c>
       <c r="B18" t="str">
         <f>IF('Product Backlog'!C10=0,"",'Product Backlog'!C10)</f>
-        <v>As a customer, I want to be able to register a user account so that I can buy, share or sell used books.</v>
+        <v>As an admin, I want to reject refund requests from users, so that I can deny the refund requests</v>
       </c>
       <c r="C18" t="e">
         <f ca="1">IF(B18="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$33,$A18,C$6),NA()))</f>
@@ -3242,7 +3241,7 @@
       </c>
       <c r="B19" t="str">
         <f>IF('Product Backlog'!C11=0,"",'Product Backlog'!C11)</f>
-        <v>As a customer, I want to be able to search for books so that I can view information about the book.</v>
+        <v>As a customer, I want to checkout my shopping cart with PayPal, so I can finish my purchase</v>
       </c>
       <c r="C19" t="e">
         <f ca="1">IF(B19="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$33,$A19,C$6),NA()))</f>
@@ -3272,7 +3271,7 @@
       </c>
       <c r="B20" t="str">
         <f>IF('Product Backlog'!C13=0,"",'Product Backlog'!C13)</f>
-        <v>As an Admin, I want to login to my admin account so that I can access my admin profile.</v>
+        <v>As a customer, I want to put items to shopping cart, so I can buy them later</v>
       </c>
       <c r="C20" t="e">
         <f ca="1">IF(B20="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$33,$A20,C$6),NA()))</f>
@@ -3332,7 +3331,7 @@
       </c>
       <c r="B22" t="str">
         <f>IF('Product Backlog'!C16=0,"",'Product Backlog'!C16)</f>
-        <v>As a business user, I want to be able to see all previous transactions, so I know how often transactions are happening.</v>
+        <v>As a customer, I want to cancel my order after 2 hours of purchasing, so I can get a full refund.</v>
       </c>
       <c r="C22" t="e">
         <f ca="1">IF(B22="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$33,$A22,C$6),NA()))</f>
@@ -3362,7 +3361,7 @@
       </c>
       <c r="B23" t="str">
         <f>IF('Product Backlog'!C17=0,"",'Product Backlog'!C17)</f>
-        <v>As a business user, I want to be able to edit the books I am managing, so I can fix mistakes when originally created the book page. </v>
+        <v>As a business user, I want to be able to upload images to my books, so that I can display previews for each book item.</v>
       </c>
       <c r="C23" t="e">
         <f ca="1">IF(B23="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$33,$A23,C$6),NA()))</f>
@@ -3392,7 +3391,7 @@
       </c>
       <c r="B24" t="str">
         <f>IF('Product Backlog'!C18=0,"",'Product Backlog'!C18)</f>
-        <v>As a customer, I want to view the details of the book I am thinking of buying, so I can be more informed on my decision.</v>
+        <v>As an admin, I want to sort all pending registrations from business users so I can view the oldest one first.</v>
       </c>
       <c r="C24" t="e">
         <f ca="1">IF(B24="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$33,$A24,C$6),NA()))</f>
@@ -3422,7 +3421,7 @@
       </c>
       <c r="B25" t="str">
         <f>IF('Product Backlog'!C20=0,"",'Product Backlog'!C20)</f>
-        <v>As an Admin, I want to see the transaction history of an item so I know if the right amount of money is being transferred</v>
+        <v>As a business user, I want to see the total amount of transactions, so I know if I am selling a large amount of books.</v>
       </c>
       <c r="C25" t="e">
         <f ca="1">IF(B25="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$33,$A25,C$6),NA()))</f>
@@ -3482,7 +3481,7 @@
       </c>
       <c r="B27" t="str">
         <f>IF('Product Backlog'!C22=0,"",'Product Backlog'!C22)</f>
-        <v>As an admin, I want to approve refund requests from users, so that I can allow the refund to the processed</v>
+        <v>As a business user, I want to know how much inventory I have left on an item, so I can decide if I need to print more books.</v>
       </c>
       <c r="C27" t="e">
         <f ca="1">IF(B27="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$33,$A27,C$6),NA()))</f>
@@ -3512,7 +3511,7 @@
       </c>
       <c r="B28" t="str">
         <f>IF('Product Backlog'!C24=0,"",'Product Backlog'!C24)</f>
-        <v>As an admin, I want to approve a pending registration from a business user so that they can open a new business account.</v>
+        <v>As a customer, I want to be able to filter my search results so that I can view only new books for sale.</v>
       </c>
       <c r="C28" t="e">
         <f ca="1">IF(B28="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$33,$A28,C$6),NA()))</f>
@@ -3602,7 +3601,7 @@
       </c>
       <c r="B31" t="str">
         <f>IF('Product Backlog'!C25=0,"",'Product Backlog'!C25)</f>
-        <v>As an admin, I want to reject a pending registration from a business user so that they are unable to open a new business account.</v>
+        <v>As a customer, I want to be able to filter my search results so that I can view only used books for sale.</v>
       </c>
       <c r="C31" t="e">
         <f ca="1">IF(B31="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$33,$A31,C$6),NA()))</f>
@@ -3632,7 +3631,7 @@
       </c>
       <c r="B32" t="str">
         <f>IF('Product Backlog'!C26=0,"",'Product Backlog'!C26)</f>
-        <v>As an admin, I want to sort all pending registrations from business users so I can view the oldest one first.</v>
+        <v>As a customer, I want to add a review to a user who sold an item to me, so I can rate the seller.</v>
       </c>
       <c r="C32" t="e">
         <f ca="1">IF(B32="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$33,$A32,C$6),NA()))</f>
@@ -3722,7 +3721,7 @@
       </c>
       <c r="B35" t="str">
         <f>IF('Product Backlog'!C15=0,"",'Product Backlog'!C15)</f>
-        <v>As a Customer, I want to create an account so I can peruse and purchase items</v>
+        <v>As a customer, I want to book items in advance, so I can get the book later when it is available.</v>
       </c>
       <c r="C35" t="e">
         <f ca="1">IF(B35="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$33,$A35,C$6),NA()))</f>
@@ -3752,7 +3751,7 @@
       </c>
       <c r="B36" t="str">
         <f>IF('Product Backlog'!C32=0,"",'Product Backlog'!C32)</f>
-        <v xml:space="preserve">As an Admin, I want to be able to add stock for a book, so that sellers can add stock to any books in their inventory. </v>
+        <v>As an Admin, I want to add new books, so that new items can be sold.</v>
       </c>
       <c r="C36" t="e">
         <f ca="1">IF(B36="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$33,$A36,C$6),NA()))</f>
@@ -3782,7 +3781,7 @@
       </c>
       <c r="B37" t="str">
         <f>IF('Product Backlog'!C33=0,"",'Product Backlog'!C33)</f>
-        <v>As a business user, I want to be able to register a business account so that I can sell and rent my books to customers.</v>
+        <v>As a Customer, I want to be able to view my transaction history, so that I can see all my recently bought books</v>
       </c>
       <c r="C37" t="e">
         <f ca="1">IF(B37="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$33,$A37,C$6),NA()))</f>
@@ -3812,7 +3811,7 @@
       </c>
       <c r="B38" t="str">
         <f>IF('Product Backlog'!C34=0,"",'Product Backlog'!C34)</f>
-        <v>As a business user, I want to be able to upload an item to sell, so that an admin can approve it.</v>
+        <v>As a business user, I want to be able to see all previous transactions, so I know how often transactions are happening.</v>
       </c>
       <c r="C38" t="e">
         <f ca="1">IF(B38="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$33,$A38,C$6),NA()))</f>
@@ -3842,7 +3841,7 @@
       </c>
       <c r="B39" t="str">
         <f>IF('Product Backlog'!C35=0,"",'Product Backlog'!C35)</f>
-        <v>As a business user, I want to export a CSV of transactions, so I know if the business is making a profit</v>
+        <v>As a business user, I want to be able to edit the books I am managing, so I can fix mistakes when originally created the book page. </v>
       </c>
       <c r="C39" t="e">
         <f ca="1">IF(B39="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$33,$A39,C$6),NA()))</f>
@@ -3872,21 +3871,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BD6B7AE05836784DB9DDF79838E135B0" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="56f2e1d40083bc882c879fd5f0e30a2e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1977bc59-59cf-46de-bb10-abef6dc3255c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="917e586b705a352b9e3a8a8ba2891683" ns2:_="">
     <xsd:import namespace="1977bc59-59cf-46de-bb10-abef6dc3255c"/>
@@ -4058,24 +4042,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8ADFF293-6F22-4BB5-9DD4-DAD0380BCBA8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3098D5BA-E904-47F9-B39A-590737902145}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48B244D2-5DBE-48D2-8344-E387AB8F9F12}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4091,4 +4073,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3098D5BA-E904-47F9-B39A-590737902145}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8ADFF293-6F22-4BB5-9DD4-DAD0380BCBA8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added final project report draft and burndown chart for sprint 3
</commit_message>
<xml_diff>
--- a/Scrum/Product Backlog.xlsx
+++ b/Scrum/Product Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jared\Desktop\SEPT\Scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7DF76D-8728-49EE-94DE-97577E933E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{521B6BCB-9262-4B91-BD1A-D535CA497BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1203,8 +1203,8 @@
   </sheetPr>
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -1316,7 +1316,7 @@
         <v>5</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H6" s="16" t="s">
         <v>13</v>
@@ -1343,7 +1343,7 @@
         <v>3</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H7" s="16" t="s">
         <v>13</v>
@@ -1368,7 +1368,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H8" s="16" t="s">
         <v>13</v>
@@ -1393,7 +1393,7 @@
         <v>3</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H9" s="16" t="s">
         <v>13</v>
@@ -1418,7 +1418,7 @@
         <v>3</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H10" s="16" t="s">
         <v>13</v>
@@ -1443,7 +1443,7 @@
         <v>13</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H11" s="16" t="s">
         <v>13</v>
@@ -1470,7 +1470,7 @@
         <v>5</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H12" s="16" t="s">
         <v>13</v>
@@ -1497,7 +1497,7 @@
         <v>5</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H13" s="16" t="s">
         <v>13</v>
@@ -1524,7 +1524,7 @@
         <v>5</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H14" s="16" t="s">
         <v>13</v>
@@ -1551,7 +1551,7 @@
         <v>3</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H15" s="16" t="s">
         <v>13</v>
@@ -1578,7 +1578,7 @@
         <v>5</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H16" s="16" t="s">
         <v>13</v>
@@ -1603,7 +1603,7 @@
         <v>13</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H17" s="16" t="s">
         <v>13</v>
@@ -1628,7 +1628,7 @@
         <v>3</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H18" s="16" t="s">
         <v>13</v>
@@ -1653,7 +1653,7 @@
         <v>8</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H19" s="16" t="s">
         <v>13</v>
@@ -1678,7 +1678,7 @@
         <v>8</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H20" s="16" t="s">
         <v>13</v>
@@ -1703,7 +1703,7 @@
         <v>8</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H21" s="16" t="s">
         <v>13</v>
@@ -1728,7 +1728,7 @@
         <v>5</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H22" s="16" t="s">
         <v>13</v>
@@ -1753,7 +1753,7 @@
         <v>3</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H23" s="16" t="s">
         <v>13</v>
@@ -1778,7 +1778,7 @@
         <v>3</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H24" s="16" t="s">
         <v>13</v>
@@ -1805,7 +1805,7 @@
         <v>3</v>
       </c>
       <c r="G25" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H25" s="16" t="s">
         <v>13</v>
@@ -1832,7 +1832,7 @@
         <v>5</v>
       </c>
       <c r="G26" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H26" s="16" t="s">
         <v>13</v>
@@ -1859,7 +1859,7 @@
         <v>5</v>
       </c>
       <c r="G27" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H27" s="16" t="s">
         <v>13</v>
@@ -1886,7 +1886,7 @@
         <v>3</v>
       </c>
       <c r="G28" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H28" s="16" t="s">
         <v>13</v>
@@ -1911,7 +1911,7 @@
         <v>3</v>
       </c>
       <c r="G29" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H29" s="16" t="s">
         <v>13</v>
@@ -1936,7 +1936,7 @@
         <v>3</v>
       </c>
       <c r="G30" s="16" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H30" s="16" t="s">
         <v>13</v>
@@ -3895,21 +3895,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BD6B7AE05836784DB9DDF79838E135B0" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="56f2e1d40083bc882c879fd5f0e30a2e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1977bc59-59cf-46de-bb10-abef6dc3255c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="917e586b705a352b9e3a8a8ba2891683" ns2:_="">
     <xsd:import namespace="1977bc59-59cf-46de-bb10-abef6dc3255c"/>
@@ -4081,24 +4066,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8ADFF293-6F22-4BB5-9DD4-DAD0380BCBA8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3098D5BA-E904-47F9-B39A-590737902145}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48B244D2-5DBE-48D2-8344-E387AB8F9F12}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4114,4 +4097,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3098D5BA-E904-47F9-B39A-590737902145}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8ADFF293-6F22-4BB5-9DD4-DAD0380BCBA8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>